<commit_message>
resolve multi insert bug of index issue
</commit_message>
<xml_diff>
--- a/Onyx/wwwroot/formats/Emp_Variable_Pay_Compoments_Import_Sample.xlsx
+++ b/Onyx/wwwroot/formats/Emp_Variable_Pay_Compoments_Import_Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HRMS\Onyx\Onyx\wwwroot\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487A90A8-612A-42FA-9147-410AF66790DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81660DC-A364-4040-BA69-A582620A4042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4464" yWindow="2172" windowWidth="17280" windowHeight="8880" xr2:uid="{E50CF398-DA2C-4B7D-84AE-DC8FC7B7A6A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E50CF398-DA2C-4B7D-84AE-DC8FC7B7A6A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Amount</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Employee Code</t>
+  </si>
+  <si>
+    <t>Narration</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92D37F5-C413-492A-8409-C5A87453E139}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -422,7 +427,9 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>

</xml_diff>